<commit_message>
bug and design: all dates bug solved and date format changed for plans page
</commit_message>
<xml_diff>
--- a/input/Aylık Plan.xlsx
+++ b/input/Aylık Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Görev</t>
   </si>
@@ -49,10 +49,10 @@
     <t>Oyun projesinin ilk kodlarının yazılması</t>
   </si>
   <si>
-    <t>20.6.2023</t>
-  </si>
-  <si>
-    <t>30.6.2023</t>
+    <t>20.06.2023</t>
+  </si>
+  <si>
+    <t>30.06.2023</t>
   </si>
   <si>
     <t>Utku Atasoy</t>
@@ -64,10 +64,7 @@
     <t>Yapay Zeka Kulübü söyleşisinin yapılması</t>
   </si>
   <si>
-    <t>20.06.2023</t>
-  </si>
-  <si>
-    <t>8.5.2023</t>
+    <t>05.08.2023</t>
   </si>
   <si>
     <t>Deniz Yıldırım</t>
@@ -81,11 +78,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -104,6 +101,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -126,25 +138,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,6 +169,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -173,14 +192,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -197,52 +208,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,187 +254,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,9 +513,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,26 +539,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -569,138 +566,138 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1025,7 +1022,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1095,16 +1092,16 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="4:4">

</xml_diff>

<commit_message>
design, statics: logos and radio button changed, static files modified
</commit_message>
<xml_diff>
--- a/input/Aylık Plan.xlsx
+++ b/input/Aylık Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Görev</t>
   </si>
@@ -31,46 +31,64 @@
     <t>Detay</t>
   </si>
   <si>
-    <t>Her kulüp adına en az bir etkinlik düzenlenmesi</t>
+    <t xml:space="preserve">Binance ile ortak bir eğitim </t>
   </si>
   <si>
     <t>01.07.2023</t>
   </si>
   <si>
-    <t>31.07.2023</t>
-  </si>
-  <si>
-    <t>Sabri Pişkin</t>
-  </si>
-  <si>
-    <t>5 Kulübün her biri online ya da offline bir etkinlik düzenleyecek</t>
-  </si>
-  <si>
-    <t>Oyun projesinin ilk kodlarının yazılması</t>
-  </si>
-  <si>
-    <t>20.06.2023</t>
-  </si>
-  <si>
-    <t>30.06.2023</t>
-  </si>
-  <si>
-    <t>Utku Atasoy</t>
-  </si>
-  <si>
-    <t>Topluluk github hesabında oyun kulübü projesi için ilk kodlar yazılacak</t>
-  </si>
-  <si>
-    <t>Yapay Zeka Kulübü söyleşisinin yapılması</t>
-  </si>
-  <si>
-    <t>05.08.2023</t>
-  </si>
-  <si>
-    <t>Deniz Yıldırım</t>
-  </si>
-  <si>
-    <t>Yapay Zeka konusunda öğrencilerin de aktif olarak katılabileceği bir söyleşi yapılacak</t>
+    <t>01.08.2023</t>
+  </si>
+  <si>
+    <t>Blockchain Kulübü</t>
+  </si>
+  <si>
+    <t>Binance'in üniversiteler ekibi ile iletişime geçilip bir blockchain dalı üzerine workshop düzenlenecek</t>
+  </si>
+  <si>
+    <t>Sektörden bir uzman ile webinar</t>
+  </si>
+  <si>
+    <t>10.07.2023</t>
+  </si>
+  <si>
+    <t>20.07.2023</t>
+  </si>
+  <si>
+    <t>Oyun Geliştirme Kulübü</t>
+  </si>
+  <si>
+    <t>Oyun geliştirme sektöründe tecrübesi bulunan bir uzman ile webinar düzenlenecek</t>
+  </si>
+  <si>
+    <t>Yapay zekanın geleceği söyleşisi</t>
+  </si>
+  <si>
+    <t>15.07.2023</t>
+  </si>
+  <si>
+    <t>Yapay Zeka Kulübü</t>
+  </si>
+  <si>
+    <t>Yapay Zekanın Geleceği konusunda öğrencilerin de aktif olarak katılabileceği bir söyleşi yapılacak</t>
+  </si>
+  <si>
+    <t>Sektörden bir uzman ile eğitim</t>
+  </si>
+  <si>
+    <t>Uygulama Geliştirme Kulübü</t>
+  </si>
+  <si>
+    <t>Uygulama geliştirme sektöründe tecrübesi bulunan bir uzman ile temel seviye bir Git eğitimi düzenlenecek</t>
+  </si>
+  <si>
+    <t>Labris Network ile söyleşi</t>
+  </si>
+  <si>
+    <t>Siber Güvenlik Kulübü</t>
+  </si>
+  <si>
+    <t>Labris Network ile siber güvenlik alanındaki fırsatların konuşulacağı bir söyleşi</t>
   </si>
 </sst>
 </file>
@@ -78,9 +96,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -101,6 +119,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -110,9 +143,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -124,13 +164,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,7 +181,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,14 +203,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -192,6 +218,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -200,6 +234,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -207,37 +256,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -254,187 +272,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,11 +466,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,43 +546,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,7 +566,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -566,130 +584,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1022,7 +1040,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1092,10 +1110,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>17</v>
@@ -1104,11 +1122,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="4:4">
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="4:4">
-      <c r="D6" s="5"/>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="4:4">
       <c r="D7" s="5"/>

</xml_diff>